<commit_message>
add results for 4p & add tests for 8p
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LM2P\Documents\000_TTU_UT\Euroteq\Distributed &amp; Parallel Computing\apm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5208989-C879-4EC2-8D74-24384249B066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6391CF4-CAD9-415C-860D-854E35AA5B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-10428" yWindow="8544" windowWidth="17280" windowHeight="8976" xr2:uid="{DE9C4FAA-FE23-4741-8F2C-7B77D437BC47}"/>
   </bookViews>
@@ -461,9 +461,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1F5605-5B40-4E95-A326-20DE76CB0444}">
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1094,11 +1094,20 @@
       <c r="E32" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="I32" s="5">
+        <v>44</v>
+      </c>
+      <c r="J32" s="5">
+        <v>43.18</v>
+      </c>
+      <c r="K32" s="5">
+        <v>43.28</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" s="6"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" s="6"/>
       <c r="C34" s="1">
         <v>2</v>
@@ -1109,8 +1118,14 @@
       <c r="E34" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J34" s="5">
+        <v>21.72</v>
+      </c>
+      <c r="K34" s="5">
+        <v>21.61</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" s="6"/>
       <c r="C35" s="1">
         <v>3</v>
@@ -1121,8 +1136,14 @@
       <c r="E35" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J35">
+        <v>10.8</v>
+      </c>
+      <c r="K35">
+        <v>10.82</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" s="6"/>
       <c r="C36" s="1">
         <v>5</v>
@@ -1133,8 +1154,14 @@
       <c r="E36" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J36" s="5">
+        <v>10.83</v>
+      </c>
+      <c r="K36" s="5">
+        <v>5.58</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" s="6"/>
       <c r="C37" s="1">
         <v>9</v>
@@ -1145,8 +1172,14 @@
       <c r="E37" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J37">
+        <v>10.58</v>
+      </c>
+      <c r="K37">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" s="6"/>
       <c r="C38" s="1">
         <v>17</v>
@@ -1157,11 +1190,17 @@
       <c r="E38" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J38" s="5">
+        <v>10.82</v>
+      </c>
+      <c r="K38" s="5">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B39" s="6"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B40" s="6"/>
       <c r="C40" s="1">
         <v>2</v>
@@ -1172,8 +1211,14 @@
       <c r="E40" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J40" s="5">
+        <v>21.81</v>
+      </c>
+      <c r="K40" s="5">
+        <v>21.77</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B41" s="6"/>
       <c r="C41" s="1">
         <v>2</v>
@@ -1184,8 +1229,14 @@
       <c r="E41" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J41">
+        <v>9.48</v>
+      </c>
+      <c r="K41">
+        <v>9.58</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B42" s="6"/>
       <c r="C42" s="1">
         <v>2</v>
@@ -1196,8 +1247,14 @@
       <c r="E42" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J42" s="5">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="K42" s="5">
+        <v>9.7100000000000009</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B43" s="6"/>
       <c r="C43" s="1">
         <v>2</v>
@@ -1208,8 +1265,14 @@
       <c r="E43" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J43">
+        <v>2.39</v>
+      </c>
+      <c r="K43">
+        <v>9.68</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B44" s="6"/>
       <c r="C44" s="1">
         <v>2</v>
@@ -1220,8 +1283,14 @@
       <c r="E44" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J44" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="K44" s="5">
+        <v>9.51</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B45" s="6"/>
       <c r="C45" s="1">
         <v>2</v>
@@ -1232,8 +1301,14 @@
       <c r="E45" s="1">
         <v>48</v>
       </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J45">
+        <v>0.95</v>
+      </c>
+      <c r="K45">
+        <v>9.68</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B47" s="6">
         <v>8</v>
       </c>
@@ -1247,7 +1322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B48" s="6"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
finish 8 pattern tests
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LM2P\Documents\000_TTU_UT\Euroteq\Distributed &amp; Parallel Computing\apm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6391CF4-CAD9-415C-860D-854E35AA5B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5211F044-DC16-4340-8685-617AF8000A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10428" yWindow="8544" windowWidth="17280" windowHeight="8976" xr2:uid="{DE9C4FAA-FE23-4741-8F2C-7B77D437BC47}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE9C4FAA-FE23-4741-8F2C-7B77D437BC47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -160,6 +160,1107 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-150"/>
+              <a:t>1</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-150" baseline="0"/>
+              <a:t> pattern</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sequential</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.99</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.99</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-620C-4801-A398-AADA9A5AF088}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Patterns over ranks</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>11.21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>9.92</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>9.91</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>9.92</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>9.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-620C-4801-A398-AADA9A5AF088}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>DB over ranks</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>11.12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.53</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>1.39</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-620C-4801-A398-AADA9A5AF088}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1072411199"/>
+        <c:axId val="1072411615"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1072411199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1072411615"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1072411615"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1072411199"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C784240E-619E-415B-B601-6C695963FEC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -462,8 +1563,8 @@
   <dimension ref="A1:N60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J46" sqref="J46"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I55" sqref="I55:I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1118,6 +2219,9 @@
       <c r="E34" s="1">
         <v>1</v>
       </c>
+      <c r="I34" s="5">
+        <v>44</v>
+      </c>
       <c r="J34" s="5">
         <v>21.72</v>
       </c>
@@ -1136,6 +2240,9 @@
       <c r="E35" s="1">
         <v>1</v>
       </c>
+      <c r="I35" s="5">
+        <v>44</v>
+      </c>
       <c r="J35">
         <v>10.8</v>
       </c>
@@ -1154,6 +2261,9 @@
       <c r="E36" s="1">
         <v>1</v>
       </c>
+      <c r="I36" s="5">
+        <v>44</v>
+      </c>
       <c r="J36" s="5">
         <v>10.83</v>
       </c>
@@ -1172,6 +2282,9 @@
       <c r="E37" s="1">
         <v>1</v>
       </c>
+      <c r="I37" s="5">
+        <v>44</v>
+      </c>
       <c r="J37">
         <v>10.58</v>
       </c>
@@ -1190,6 +2303,9 @@
       <c r="E38" s="1">
         <v>1</v>
       </c>
+      <c r="I38" s="5">
+        <v>44</v>
+      </c>
       <c r="J38" s="5">
         <v>10.82</v>
       </c>
@@ -1211,6 +2327,9 @@
       <c r="E40" s="1">
         <v>2</v>
       </c>
+      <c r="I40" s="5">
+        <v>44</v>
+      </c>
       <c r="J40" s="5">
         <v>21.81</v>
       </c>
@@ -1229,6 +2348,9 @@
       <c r="E41" s="1">
         <v>4</v>
       </c>
+      <c r="I41" s="5">
+        <v>44</v>
+      </c>
       <c r="J41">
         <v>9.48</v>
       </c>
@@ -1247,6 +2369,9 @@
       <c r="E42" s="1">
         <v>8</v>
       </c>
+      <c r="I42" s="5">
+        <v>44</v>
+      </c>
       <c r="J42" s="5">
         <v>4.7699999999999996</v>
       </c>
@@ -1265,6 +2390,9 @@
       <c r="E43" s="1">
         <v>16</v>
       </c>
+      <c r="I43" s="5">
+        <v>44</v>
+      </c>
       <c r="J43">
         <v>2.39</v>
       </c>
@@ -1283,6 +2411,9 @@
       <c r="E44" s="1">
         <v>24</v>
       </c>
+      <c r="I44" s="5">
+        <v>44</v>
+      </c>
       <c r="J44" s="5">
         <v>1.7</v>
       </c>
@@ -1301,6 +2432,9 @@
       <c r="E45" s="1">
         <v>48</v>
       </c>
+      <c r="I45" s="5">
+        <v>44</v>
+      </c>
       <c r="J45">
         <v>0.95</v>
       </c>
@@ -1321,11 +2455,20 @@
       <c r="E47" s="1">
         <v>1</v>
       </c>
+      <c r="I47" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="J47">
+        <v>86.87</v>
+      </c>
+      <c r="K47">
+        <v>86.71</v>
+      </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B48" s="6"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B49" s="6"/>
       <c r="C49" s="1">
         <v>2</v>
@@ -1336,8 +2479,17 @@
       <c r="E49" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="I49" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="J49">
+        <v>43.87</v>
+      </c>
+      <c r="K49">
+        <v>42.21</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B50" s="6"/>
       <c r="C50" s="1">
         <v>3</v>
@@ -1348,8 +2500,17 @@
       <c r="E50" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="I50" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="J50">
+        <v>21.77</v>
+      </c>
+      <c r="K50">
+        <v>21.32</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B51" s="6"/>
       <c r="C51" s="1">
         <v>5</v>
@@ -1360,8 +2521,17 @@
       <c r="E51" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="I51" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="J51">
+        <v>11.15</v>
+      </c>
+      <c r="K51">
+        <v>11.16</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B52" s="6"/>
       <c r="C52" s="1">
         <v>9</v>
@@ -1372,8 +2542,17 @@
       <c r="E52" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="I52" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="J52">
+        <v>11.14</v>
+      </c>
+      <c r="K52">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B53" s="6"/>
       <c r="C53" s="1">
         <v>17</v>
@@ -1384,11 +2563,20 @@
       <c r="E53" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="I53" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="J53">
+        <v>11.12</v>
+      </c>
+      <c r="K53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B54" s="6"/>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B55" s="6"/>
       <c r="C55" s="1">
         <v>2</v>
@@ -1399,8 +2587,17 @@
       <c r="E55" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="I55" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="J55">
+        <v>41.6</v>
+      </c>
+      <c r="K55">
+        <v>41.76</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B56" s="6"/>
       <c r="C56" s="1">
         <v>2</v>
@@ -1411,8 +2608,17 @@
       <c r="E56" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="I56" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="J56">
+        <v>18.989999999999998</v>
+      </c>
+      <c r="K56">
+        <v>19.05</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B57" s="6"/>
       <c r="C57" s="1">
         <v>2</v>
@@ -1423,8 +2629,17 @@
       <c r="E57" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="I57" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="J57">
+        <v>9.4600000000000009</v>
+      </c>
+      <c r="K57">
+        <v>9.52</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B58" s="6"/>
       <c r="C58" s="1">
         <v>2</v>
@@ -1435,8 +2650,17 @@
       <c r="E58" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="I58" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="J58">
+        <v>4.82</v>
+      </c>
+      <c r="K58">
+        <v>9.39</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B59" s="6"/>
       <c r="C59" s="1">
         <v>2</v>
@@ -1447,8 +2671,17 @@
       <c r="E59" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="I59" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="J59">
+        <v>3.37</v>
+      </c>
+      <c r="K59">
+        <v>9.52</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B60" s="6"/>
       <c r="C60" s="1">
         <v>2</v>
@@ -1458,6 +2691,15 @@
       </c>
       <c r="E60" s="1">
         <v>48</v>
+      </c>
+      <c r="I60" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="J60">
+        <v>1.87</v>
+      </c>
+      <c r="K60">
+        <v>9.3800000000000008</v>
       </c>
     </row>
   </sheetData>
@@ -1468,5 +2710,6 @@
     <mergeCell ref="B47:B60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add tests & results for big db -  4 patterns
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LM2P\Documents\000_TTU_UT\Euroteq\Distributed &amp; Parallel Computing\apm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5211F044-DC16-4340-8685-617AF8000A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA7CB14-72A4-41F0-BEC0-100BE53DD33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE9C4FAA-FE23-4741-8F2C-7B77D437BC47}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t># Nodes</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>We would expect ~0.40 s but overhead of communication begins to affect</t>
+  </si>
+  <si>
+    <t>Big</t>
   </si>
 </sst>
 </file>
@@ -378,16 +381,16 @@
                 <c:pt idx="2">
                   <c:v>9.9</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="3">
                   <c:v>9.92</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
+                <c:pt idx="4">
                   <c:v>9.91</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="5">
                   <c:v>9.92</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="6">
                   <c:v>9.92</c:v>
                 </c:pt>
               </c:numCache>
@@ -457,16 +460,16 @@
                 <c:pt idx="2">
                   <c:v>5.53</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="3">
                   <c:v>2.75</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
+                <c:pt idx="4">
                   <c:v>1.39</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="5">
                   <c:v>0.79</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="6">
                   <c:v>0.56000000000000005</c:v>
                 </c:pt>
               </c:numCache>
@@ -1233,9 +1236,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1560,11 +1563,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1F5605-5B40-4E95-A326-20DE76CB0444}">
-  <dimension ref="A1:N60"/>
+  <dimension ref="A1:N69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I55" sqref="I55:I60"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L69" sqref="L69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1616,7 +1619,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="6">
@@ -1648,12 +1651,14 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="1">
         <v>2</v>
@@ -1684,6 +1689,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="1">
         <v>3</v>
@@ -1700,14 +1706,15 @@
       <c r="I5" s="5">
         <v>10.99</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="5">
         <v>9.92</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="5">
         <v>2.75</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="1">
         <v>5</v>
@@ -1721,14 +1728,15 @@
       <c r="I6" s="5">
         <v>10.99</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="5">
         <v>9.91</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="5">
         <v>1.39</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="1">
         <v>9</v>
@@ -1742,10 +1750,10 @@
       <c r="I7" s="5">
         <v>10.99</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="5">
         <v>9.92</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="5">
         <v>0.79</v>
       </c>
       <c r="N7" t="s">
@@ -1753,6 +1761,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="1">
         <v>17</v>
@@ -1766,10 +1775,10 @@
       <c r="I8" s="5">
         <v>10.99</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="5">
         <v>9.92</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="5">
         <v>0.56000000000000005</v>
       </c>
       <c r="N8" t="s">
@@ -1777,9 +1786,14 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
       <c r="B9" s="6"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="1">
         <v>2</v>
@@ -1796,11 +1810,12 @@
       <c r="J10" s="5">
         <v>5.63</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="5">
         <v>11.12</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="1">
         <v>2</v>
@@ -1814,14 +1829,15 @@
       <c r="I11" s="5">
         <v>10.99</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="5">
         <v>2.37</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="5">
         <v>11.17</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="1">
         <v>2</v>
@@ -1835,14 +1851,15 @@
       <c r="I12" s="5">
         <v>10.99</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="5">
         <v>1.21</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="5">
         <v>11.05</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="1">
         <v>2</v>
@@ -1856,14 +1873,15 @@
       <c r="I13" s="5">
         <v>10.99</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="5">
         <v>0.63</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="5">
         <v>11.12</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="1">
         <v>2</v>
@@ -1877,14 +1895,15 @@
       <c r="I14" s="5">
         <v>10.99</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="5">
         <v>0.44</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="5">
         <v>11.15</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="1">
         <v>2</v>
@@ -1898,14 +1917,21 @@
       <c r="I15" s="5">
         <v>10.99</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="5">
         <v>0.25</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="5">
         <v>11.2</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
       <c r="B17" s="6">
         <v>2</v>
       </c>
@@ -1934,7 +1960,8 @@
         <v>21.85</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="I18" s="5">
         <v>22.04</v>
@@ -1942,7 +1969,8 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="1">
         <v>2</v>
@@ -1966,7 +1994,8 @@
         <v>11.17</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="1">
         <v>3</v>
@@ -1990,7 +2019,8 @@
         <v>5.5209999999999999</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="1">
         <v>5</v>
@@ -2011,7 +2041,8 @@
         <v>2.81</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="1">
         <v>9</v>
@@ -2032,7 +2063,8 @@
         <v>1.46</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="1">
         <v>17</v>
@@ -2053,10 +2085,15 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="6"/>
       <c r="B24" s="6"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="1">
         <v>2</v>
@@ -2077,7 +2114,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="1">
         <v>2</v>
@@ -2098,7 +2136,8 @@
         <v>11.06</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="1">
         <v>2</v>
@@ -2119,7 +2158,8 @@
         <v>11.08</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="1">
         <v>2</v>
@@ -2140,7 +2180,8 @@
         <v>11.07</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="1">
         <v>2</v>
@@ -2161,7 +2202,8 @@
         <v>11.05</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="1">
         <v>2</v>
@@ -2182,7 +2224,14 @@
         <v>11.07</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="6"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="6"/>
       <c r="B32" s="6">
         <v>4</v>
       </c>
@@ -2205,10 +2254,15 @@
         <v>43.28</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="6"/>
       <c r="B33" s="6"/>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="1">
         <v>2</v>
@@ -2229,7 +2283,8 @@
         <v>21.61</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="1">
         <v>3</v>
@@ -2243,14 +2298,15 @@
       <c r="I35" s="5">
         <v>44</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="5">
         <v>10.8</v>
       </c>
-      <c r="K35">
+      <c r="K35" s="5">
         <v>10.82</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="1">
         <v>5</v>
@@ -2271,7 +2327,8 @@
         <v>5.58</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="1">
         <v>9</v>
@@ -2285,14 +2342,15 @@
       <c r="I37" s="5">
         <v>44</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="5">
         <v>10.58</v>
       </c>
-      <c r="K37">
+      <c r="K37" s="5">
         <v>2.83</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="1">
         <v>17</v>
@@ -2313,10 +2371,15 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="6"/>
       <c r="B39" s="6"/>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="1">
         <v>2</v>
@@ -2337,7 +2400,8 @@
         <v>21.77</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="1">
         <v>2</v>
@@ -2351,14 +2415,15 @@
       <c r="I41" s="5">
         <v>44</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="5">
         <v>9.48</v>
       </c>
-      <c r="K41">
+      <c r="K41" s="5">
         <v>9.58</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="1">
         <v>2</v>
@@ -2379,7 +2444,8 @@
         <v>9.7100000000000009</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="1">
         <v>2</v>
@@ -2393,14 +2459,15 @@
       <c r="I43" s="5">
         <v>44</v>
       </c>
-      <c r="J43">
+      <c r="J43" s="5">
         <v>2.39</v>
       </c>
-      <c r="K43">
+      <c r="K43" s="5">
         <v>9.68</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="1">
         <v>2</v>
@@ -2421,7 +2488,8 @@
         <v>9.51</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="1">
         <v>2</v>
@@ -2435,14 +2503,21 @@
       <c r="I45" s="5">
         <v>44</v>
       </c>
-      <c r="J45">
+      <c r="J45" s="5">
         <v>0.95</v>
       </c>
-      <c r="K45">
+      <c r="K45" s="5">
         <v>9.68</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="6"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="6"/>
       <c r="B47" s="6">
         <v>8</v>
       </c>
@@ -2458,17 +2533,22 @@
       <c r="I47" s="5">
         <v>88.02</v>
       </c>
-      <c r="J47">
+      <c r="J47" s="5">
         <v>86.87</v>
       </c>
-      <c r="K47">
+      <c r="K47" s="5">
         <v>86.71</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="6"/>
       <c r="B48" s="6"/>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="1">
         <v>2</v>
@@ -2482,14 +2562,15 @@
       <c r="I49" s="5">
         <v>88.02</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="5">
         <v>43.87</v>
       </c>
-      <c r="K49">
+      <c r="K49" s="5">
         <v>42.21</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="1">
         <v>3</v>
@@ -2503,14 +2584,15 @@
       <c r="I50" s="5">
         <v>88.02</v>
       </c>
-      <c r="J50">
+      <c r="J50" s="5">
         <v>21.77</v>
       </c>
-      <c r="K50">
+      <c r="K50" s="5">
         <v>21.32</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="1">
         <v>5</v>
@@ -2524,14 +2606,15 @@
       <c r="I51" s="5">
         <v>88.02</v>
       </c>
-      <c r="J51">
+      <c r="J51" s="5">
         <v>11.15</v>
       </c>
-      <c r="K51">
+      <c r="K51" s="5">
         <v>11.16</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="1">
         <v>9</v>
@@ -2545,14 +2628,15 @@
       <c r="I52" s="5">
         <v>88.02</v>
       </c>
-      <c r="J52">
+      <c r="J52" s="5">
         <v>11.14</v>
       </c>
-      <c r="K52">
+      <c r="K52" s="5">
         <v>5.6</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="1">
         <v>17</v>
@@ -2566,17 +2650,22 @@
       <c r="I53" s="5">
         <v>88.02</v>
       </c>
-      <c r="J53">
+      <c r="J53" s="5">
         <v>11.12</v>
       </c>
-      <c r="K53">
+      <c r="K53" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" s="6"/>
       <c r="B54" s="6"/>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="1">
         <v>2</v>
@@ -2590,14 +2679,15 @@
       <c r="I55" s="5">
         <v>88.02</v>
       </c>
-      <c r="J55">
+      <c r="J55" s="5">
         <v>41.6</v>
       </c>
-      <c r="K55">
+      <c r="K55" s="5">
         <v>41.76</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="1">
         <v>2</v>
@@ -2611,14 +2701,15 @@
       <c r="I56" s="5">
         <v>88.02</v>
       </c>
-      <c r="J56">
+      <c r="J56" s="5">
         <v>18.989999999999998</v>
       </c>
-      <c r="K56">
+      <c r="K56" s="5">
         <v>19.05</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="1">
         <v>2</v>
@@ -2632,14 +2723,15 @@
       <c r="I57" s="5">
         <v>88.02</v>
       </c>
-      <c r="J57">
+      <c r="J57" s="5">
         <v>9.4600000000000009</v>
       </c>
-      <c r="K57">
+      <c r="K57" s="5">
         <v>9.52</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="1">
         <v>2</v>
@@ -2653,14 +2745,15 @@
       <c r="I58" s="5">
         <v>88.02</v>
       </c>
-      <c r="J58">
+      <c r="J58" s="5">
         <v>4.82</v>
       </c>
-      <c r="K58">
+      <c r="K58" s="5">
         <v>9.39</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="1">
         <v>2</v>
@@ -2674,14 +2767,15 @@
       <c r="I59" s="5">
         <v>88.02</v>
       </c>
-      <c r="J59">
+      <c r="J59" s="5">
         <v>3.37</v>
       </c>
-      <c r="K59">
+      <c r="K59" s="5">
         <v>9.52</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="1">
         <v>2</v>
@@ -2695,19 +2789,148 @@
       <c r="I60" s="5">
         <v>88.02</v>
       </c>
-      <c r="J60">
+      <c r="J60" s="5">
         <v>1.87</v>
       </c>
-      <c r="K60">
+      <c r="K60" s="5">
         <v>9.3800000000000008</v>
       </c>
     </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" s="6">
+        <v>4</v>
+      </c>
+      <c r="C62" s="1">
+        <v>2</v>
+      </c>
+      <c r="D62" s="1">
+        <v>2</v>
+      </c>
+      <c r="E62" s="1">
+        <v>1</v>
+      </c>
+      <c r="I62" s="5">
+        <v>31.73</v>
+      </c>
+      <c r="J62" s="5">
+        <v>31.75</v>
+      </c>
+      <c r="K62" s="5">
+        <v>30.13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" s="6"/>
+      <c r="B63" s="6"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" s="6"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="1">
+        <v>3</v>
+      </c>
+      <c r="D64" s="1">
+        <v>5</v>
+      </c>
+      <c r="E64" s="1">
+        <v>1</v>
+      </c>
+      <c r="I64" s="5">
+        <v>31.73</v>
+      </c>
+      <c r="J64" s="5">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="K64" s="5">
+        <v>8.02</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A65" s="6"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="1">
+        <v>17</v>
+      </c>
+      <c r="D65" s="1">
+        <v>33</v>
+      </c>
+      <c r="E65" s="1">
+        <v>1</v>
+      </c>
+      <c r="I65" s="5">
+        <v>31.73</v>
+      </c>
+      <c r="J65">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="K65">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" s="6"/>
+      <c r="B66" s="6"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A67" s="6"/>
+      <c r="B67" s="6"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" s="6"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="1">
+        <v>2</v>
+      </c>
+      <c r="D68" s="1">
+        <v>2</v>
+      </c>
+      <c r="E68" s="1">
+        <v>4</v>
+      </c>
+      <c r="I68" s="5">
+        <v>31.73</v>
+      </c>
+      <c r="J68">
+        <v>6.83</v>
+      </c>
+      <c r="K68">
+        <v>6.95</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A69" s="6"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="1">
+        <v>2</v>
+      </c>
+      <c r="D69" s="1">
+        <v>2</v>
+      </c>
+      <c r="E69" s="1">
+        <v>48</v>
+      </c>
+      <c r="I69" s="5">
+        <v>31.73</v>
+      </c>
+      <c r="J69">
+        <v>0.69</v>
+      </c>
+      <c r="K69">
+        <v>6.85</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="B62:B69"/>
+    <mergeCell ref="A62:A69"/>
     <mergeCell ref="B2:B15"/>
     <mergeCell ref="B17:B30"/>
     <mergeCell ref="B32:B45"/>
     <mergeCell ref="B47:B60"/>
+    <mergeCell ref="A2:A60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>